<commit_message>
update design and files
</commit_message>
<xml_diff>
--- a/Datasheets/gain calculation (Autosaved).xlsx
+++ b/Datasheets/gain calculation (Autosaved).xlsx
@@ -413,7 +413,7 @@
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -455,30 +455,30 @@
         <v>1E-3</v>
       </c>
       <c r="B2">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C2">
         <f>A2*B2</f>
-        <v>1.0000000000000001E-5</v>
+        <v>5.0000000000000004E-6</v>
       </c>
       <c r="D2">
         <v>8</v>
       </c>
       <c r="E2">
         <f>C2*D$2</f>
-        <v>8.0000000000000007E-5</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="F2">
         <f>C2*D$3</f>
-        <v>1.6000000000000001E-4</v>
+        <v>8.0000000000000007E-5</v>
       </c>
       <c r="G2">
         <f>C2*D$4</f>
-        <v>3.2000000000000003E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="H2" s="1">
         <f>C2*D$5</f>
-        <v>6.4000000000000005E-4</v>
+        <v>3.2000000000000003E-4</v>
       </c>
       <c r="I2">
         <f>1/4096</f>

</xml_diff>